<commit_message>
updated rubric checklist and added image ML model
</commit_message>
<xml_diff>
--- a/Resources/Rubric_Checklist_by_Segment.xlsx
+++ b/Resources/Rubric_Checklist_by_Segment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teresa\Class\Rural_Surge\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1964C6C1-2032-4F85-B5F2-16EB4A4731FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B131A4B7-BD01-4469-AC7E-659EFD05E801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0B9D832E-C2C1-4BCD-AA9C-E2B0D7255C7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{0B9D832E-C2C1-4BCD-AA9C-E2B0D7255C7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentation" sheetId="2" r:id="rId1"/>
@@ -272,94 +272,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-The presentation outlines the project, including the following:
-Selected topic
-Reason why they selected their topic
-Description of their source of data
-Questions they hope to answer with the data
-Description of the data exploration phase of the project
-Description of the analysis phase of the project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Slides</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Presentations are drafted in Google Slides</t>
-    </r>
-  </si>
-  <si>
-    <t>Team members submit the code for their machine learning model, as well as the following:
-Description of preliminary data preprocessing
-Description of preliminary feature engineering and preliminary feature selection, including their decision-making
-process
-Description of how data was split into training and testing sets
-Explanation of model choice, including limitations and benefits</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Team members present a fully integrated database.
-Database stores static data for use during the project
-Database interfaces with the project in some format (e.g., scraping updates the database, or database connects to the model)
-Includes at least two tables (or collections, if using MongoDB)
-Includes at least one join using the database language (not including any joins in Pandas)
-Includes at least one connection string (using SQLAlchemy or PyMongo)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: If you use a SQL database, you must provide your ERD with relationships</t>
-    </r>
-  </si>
-  <si>
-    <t>A blueprint for the dashboard is created and includes all of the following:
-Storyboard on Google Slide(s)
-Description of the tool(s) that will be used to create final dashboard
-Description of interactive element(s)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Content</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">: The presentation tells a story about their project, including the following:
 Selected topic
 Reason why they selected their topic
@@ -570,102 +482,6 @@
       </rPr>
       <t>Note: The descriptions and
 explanations required in all other project deliverables should also be in your README.md as part of your outline, unless otherwise noted.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Main Branch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> All code in the main branch is production ready.
-The main branch should include:
-All code necessary to perform exploratory analysis
-Some code necessary to complete the machine learning portion of the project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">README.md </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">must include:
-Description of the communication protocols
-Outline of the project (this may include images, but should be easy to follow and digest)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: The descriptions and explanations required in all other project deliverables should also be in your README.md as part of your outline, unless otherwise noted.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Individual Branches</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-At least one branch for each team member
-Each team member has at least four commits for the duration of the second segment (eight total commits per person)</t>
     </r>
   </si>
   <si>
@@ -896,12 +712,395 @@
 ✓ Submission includes speaker notes, flashcards, or a video of the presentation rehearsal</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team members submit the code for their machine learning model, as well as the following:
+Description of preliminary data preprocessing
+Description of preliminary feature engineering and preliminary feature selection, including their decision-making
+process
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Description of how data was split into training and testing sets
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Explanation of model choice, including limitations and benefits</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team members present a fully integrated database.
+Database stores static data for use during the project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Database interfaces with the project in some format (e.g., scraping updates the database, or database connects to the model)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Includes at least two tables (or collections, if using MongoDB)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Includes at least one join using the database language (not including any joins in Pandas)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Includes at least one connection string (using SQLAlchemy or PyMongo)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: If you use a SQL database, you must provide your</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ERD with relationships (revise)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The presentation outlines the project, including the following:
+Selected topic
+Reason why they selected their topic
+Description of their source of data
+Questions they hope to answer with the data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description of the data exploration phase of the project
+Description of the analysis phase of the project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Slides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Presentations are drafted in Google Slides</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Main Branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> All code in the main branch is production ready.
+The main branch should include:
+All code necessary to perform exploratory analysis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Some code necessary to complete the machine learning portion of the project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">README.md </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">must include:
+Description of the communication protocols
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Outline of the project (this may include images, but should be easy to follow and digest)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: The descriptions and explanations required in all other project deliverables should also be in your README.md as part of your outline, unless otherwise noted.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Individual Branches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+At least one branch for each team member
+Each team member has at least four commits for the duration of the second segment (eight total commits per person)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A blueprint for the dashboard is created and includes all of the following:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Storyboard on Google Slide(s)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Description of the tool(s) that will be used to create final dashboard
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description of interactive element(s)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -937,6 +1136,21 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1089,56 +1303,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1146,20 +1312,131 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1167,24 +1444,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,18 +1453,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1214,39 +1461,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,10 +1781,10 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection activeCell="D2" sqref="D2:D17"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1579,236 +1793,236 @@
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="40.33203125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" customWidth="1"/>
     <col min="6" max="6" width="30.6640625" customWidth="1"/>
     <col min="7" max="7" width="45.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="56" t="s">
+      <c r="D2" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>83</v>
+      <c r="G2" s="19" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="44" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="45" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="44" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="45" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="44" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="45" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="50" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="44" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="45" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="44" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="45" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="50" t="s">
+      <c r="A17" s="27"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1837,10 +2051,10 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection activeCell="C4" sqref="C4"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection pane="topRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1849,166 +2063,167 @@
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="38.109375" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.77734375" customWidth="1"/>
+    <col min="5" max="5" width="48.44140625" customWidth="1"/>
     <col min="6" max="6" width="38.5546875" customWidth="1"/>
     <col min="7" max="7" width="44.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="45" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="27"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="27"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="43"/>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="54" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="27"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="43"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="97.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="50" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="27"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="43"/>
     </row>
     <row r="9" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="27"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="43"/>
     </row>
     <row r="10" spans="1:7" ht="83.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="50" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="28"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="8" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A2:A10"/>
     <mergeCell ref="D2:D10"/>
     <mergeCell ref="E2:E10"/>
     <mergeCell ref="F2:F10"/>
@@ -2016,7 +2231,6 @@
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A10"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
   <pageSetup scale="54" orientation="landscape" r:id="rId1"/>
@@ -2033,10 +2247,10 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection activeCell="C4" sqref="C4"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2045,157 +2259,157 @@
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="41.88671875" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="29.5546875" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" customWidth="1"/>
     <col min="7" max="7" width="33.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="45" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>82</v>
+      <c r="E2" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2223,10 +2437,10 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection activeCell="C4" sqref="C4"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2235,113 +2449,113 @@
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" customWidth="1"/>
-    <col min="5" max="5" width="32.77734375" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" customWidth="1"/>
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="40" t="s">
+      <c r="E2" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="37" t="s">
-        <v>81</v>
+      <c r="G2" s="19" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="44" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="38"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="38"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="38"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="46" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="39"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2369,10 +2583,10 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection activeCell="C4" sqref="C4"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2387,96 +2601,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>80</v>
+      <c r="E2" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="44" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="99.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="50" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="8" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated checklist and schema
</commit_message>
<xml_diff>
--- a/Resources/Rubric_Checklist_by_Segment.xlsx
+++ b/Resources/Rubric_Checklist_by_Segment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teresa\Class\Rural_Surge\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B131A4B7-BD01-4469-AC7E-659EFD05E801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559D5E30-C49C-464C-A02A-1DDDF320AC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{0B9D832E-C2C1-4BCD-AA9C-E2B0D7255C7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0B9D832E-C2C1-4BCD-AA9C-E2B0D7255C7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentation" sheetId="2" r:id="rId1"/>
@@ -921,6 +921,44 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">A blueprint for the dashboard is created and includes all of the following:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Storyboard on Google Slide(s)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Description of the tool(s) that will be used to create final dashboard
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description of interactive element(s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -991,13 +1029,24 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Outline of the project (this may include images, but should be easy to follow and digest)</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Outline of the project (this may include images, but should be easy to follow and digest)
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -1055,44 +1104,6 @@
       <t xml:space="preserve">
 At least one branch for each team member
 Each team member has at least four commits for the duration of the second segment (eight total commits per person)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A blueprint for the dashboard is created and includes all of the following:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Storyboard on Google Slide(s)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Description of the tool(s) that will be used to create final dashboard
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Description of interactive element(s)</t>
     </r>
   </si>
 </sst>
@@ -1100,7 +1111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1151,6 +1162,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1784,7 +1803,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="E2" sqref="E2:E17"/>
-      <selection pane="topRight" activeCell="G2" sqref="G2:G17"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2054,7 +2073,7 @@
     <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="E2" sqref="E2:E17"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2105,7 +2124,7 @@
         <v>69</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>68</v>
@@ -2247,8 +2266,8 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="E2" sqref="E2:E17"/>
       <selection pane="topRight" activeCell="E2" sqref="E2:E10"/>
     </sheetView>
@@ -2437,10 +2456,10 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="E2" sqref="E2:E17"/>
-      <selection pane="topRight" activeCell="F2" sqref="F2:F6"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2583,10 +2602,10 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="E2" sqref="E2:E17"/>
-      <selection pane="topRight" activeCell="F2" sqref="F2:F5"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2637,7 +2656,7 @@
         <v>66</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>71</v>

</xml_diff>